<commit_message>
adding a pep725_direct configuration
</commit_message>
<xml_diff>
--- a/docs/ReasonerPerformanceTest.xlsx
+++ b/docs/ReasonerPerformanceTest.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>Reasoner</t>
   </si>
@@ -50,15 +50,6 @@
     <t>mini</t>
   </si>
   <si>
-    <t>plantStructure/measurementDatum instances and all annotations</t>
-  </si>
-  <si>
-    <t>plantStructure/measurementDatum instances and minimal annotations</t>
-  </si>
-  <si>
-    <t>all class instances and all annotations</t>
-  </si>
-  <si>
     <t>seconds inferred</t>
   </si>
   <si>
@@ -90,14 +81,40 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>Contains only two classes: plantStructurePresence and measurementDatum. Only the Datatype properties are included here that are absolutely necessary for inferencing to happen (counts and percents) are contained these classes.</t>
+  </si>
+  <si>
+    <t>overall seconds / triple</t>
+  </si>
+  <si>
+    <t>Contains only two classes: plantStructurePresence and measurementDatum. Most of the Annotation properties from the source data are contained these classes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contains a full set of classes, relations between classes, and all of the annotations needed to describe the data. </t>
+  </si>
+  <si>
+    <t>triples / record</t>
+  </si>
+  <si>
+    <t>NOTE: tests conducted on a Mac OS X with 8Gb RAM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,9 +142,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -407,543 +426,689 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="I10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="K10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11">
         <v>1000</v>
       </c>
-      <c r="D9">
+      <c r="D11">
         <v>9902</v>
       </c>
-      <c r="E9">
+      <c r="E11">
+        <f t="shared" ref="E11:E15" si="0">D11/C11</f>
+        <v>9.9019999999999992</v>
+      </c>
+      <c r="F11">
         <f>96*60</f>
         <v>5760</v>
       </c>
-      <c r="F9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12">
         <v>100</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>1023</v>
       </c>
-      <c r="E10">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>10.23</v>
+      </c>
+      <c r="F12">
         <v>345</v>
       </c>
-      <c r="F10">
+      <c r="G12">
         <v>1523</v>
       </c>
-      <c r="G10">
+      <c r="H12">
         <f>(31*60)+27</f>
         <v>1887</v>
       </c>
-      <c r="H10">
-        <f>G10/C10</f>
+      <c r="I12">
+        <f>H12/C12</f>
         <v>18.87</v>
       </c>
-      <c r="I10">
-        <f>(H10*500000)/60/60/24/30</f>
+      <c r="J12" s="1">
+        <f t="shared" ref="J12:J15" si="1">H12/D12</f>
+        <v>1.8445747800586509</v>
+      </c>
+      <c r="K12">
+        <f>(I12*500000)/60/60/24/30</f>
         <v>3.6400462962962967</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11">
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13">
         <v>50</v>
       </c>
-      <c r="D11">
+      <c r="D13">
         <v>538</v>
       </c>
-      <c r="E11">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>10.76</v>
+      </c>
+      <c r="F13">
         <v>264</v>
       </c>
-      <c r="F11">
+      <c r="G13">
         <v>1166</v>
       </c>
-      <c r="G11">
+      <c r="H13">
         <f>(24*60)+10</f>
         <v>1450</v>
       </c>
-      <c r="H11">
-        <f>G11/C11</f>
+      <c r="I13">
+        <f>H13/C13</f>
         <v>29</v>
       </c>
-      <c r="I11">
-        <f>(H11*500000)/60/60/24/30</f>
+      <c r="J13" s="1">
+        <f t="shared" si="1"/>
+        <v>2.6951672862453533</v>
+      </c>
+      <c r="K13">
+        <f>(I13*500000)/60/60/24/30</f>
         <v>5.5941358024691361</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14">
         <v>10</v>
       </c>
-      <c r="D12">
+      <c r="D14">
         <v>144</v>
       </c>
-      <c r="E12">
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>14.4</v>
+      </c>
+      <c r="F14">
         <v>64</v>
       </c>
-      <c r="F12">
+      <c r="G14">
         <v>1.89</v>
       </c>
-      <c r="G12">
+      <c r="H14">
         <v>83</v>
       </c>
-      <c r="H12">
-        <f>G12/C12</f>
+      <c r="I14">
+        <f>H14/C14</f>
         <v>8.3000000000000007</v>
       </c>
-      <c r="I12">
-        <f>(H12*500000)/60/60/24/30</f>
+      <c r="J14" s="1">
+        <f t="shared" si="1"/>
+        <v>0.57638888888888884</v>
+      </c>
+      <c r="K14">
+        <f>(I14*500000)/60/60/24/30</f>
         <v>1.6010802469135803</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
         <v>45</v>
       </c>
-      <c r="E13">
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="F15">
         <v>18</v>
       </c>
-      <c r="F13">
+      <c r="G15">
         <v>0.41899999999999998</v>
       </c>
-      <c r="G13">
+      <c r="H15">
         <v>36</v>
       </c>
-      <c r="H13">
-        <f>G13/C13</f>
+      <c r="I15">
+        <f>H15/C15</f>
         <v>36</v>
       </c>
-      <c r="I13">
-        <f>(H13*500000)/60/60/24/30</f>
+      <c r="J15" s="1">
+        <f t="shared" si="1"/>
+        <v>0.8</v>
+      </c>
+      <c r="K15">
+        <f>(I15*500000)/60/60/24/30</f>
         <v>6.9444444444444446</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15">
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
         <v>1000</v>
       </c>
-      <c r="D15">
+      <c r="D17">
         <v>9050</v>
       </c>
-      <c r="E15">
+      <c r="E17">
+        <f t="shared" ref="E17:E21" si="2">D17/C17</f>
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="F17">
         <v>7500</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" t="s">
         <v>15</v>
       </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="H15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" t="s">
-        <v>15</v>
-      </c>
-      <c r="J15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>5</v>
       </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
         <v>100</v>
       </c>
-      <c r="D16">
+      <c r="D18">
         <v>1362</v>
       </c>
-      <c r="E16">
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>13.62</v>
+      </c>
+      <c r="F18">
         <v>306</v>
       </c>
-      <c r="F16">
+      <c r="G18">
         <v>754</v>
       </c>
-      <c r="G16">
+      <c r="H18">
         <f>18*60</f>
         <v>1080</v>
       </c>
-      <c r="H16">
-        <f>G16/C16</f>
+      <c r="I18">
+        <f>H18/C18</f>
         <v>10.8</v>
       </c>
-      <c r="I16">
-        <f>(H16*500000)/60/60/24/30</f>
+      <c r="J18" s="1">
+        <f t="shared" ref="J18:J21" si="3">H18/D18</f>
+        <v>0.79295154185022021</v>
+      </c>
+      <c r="K18">
+        <f>(I18*500000)/60/60/24/30</f>
         <v>2.0833333333333335</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17">
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>50</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <v>719</v>
       </c>
-      <c r="E17">
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>14.38</v>
+      </c>
+      <c r="F19">
         <v>260</v>
       </c>
-      <c r="F17">
+      <c r="G19">
         <v>682</v>
       </c>
-      <c r="G17">
+      <c r="H19">
         <f>16*60</f>
         <v>960</v>
       </c>
-      <c r="H17">
-        <f>G17/C17</f>
+      <c r="I19">
+        <f>H19/C19</f>
         <v>19.2</v>
       </c>
-      <c r="I17">
-        <f>(H17*500000)/60/60/24/30</f>
+      <c r="J19" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3351877607788596</v>
+      </c>
+      <c r="K19">
+        <f>(I19*500000)/60/60/24/30</f>
         <v>3.7037037037037033</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>5</v>
       </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>10</v>
       </c>
-      <c r="D18">
+      <c r="D20">
         <v>205</v>
       </c>
-      <c r="E18">
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>20.5</v>
+      </c>
+      <c r="F20">
         <v>55</v>
       </c>
-      <c r="F18">
+      <c r="G20">
         <v>2.5499999999999998</v>
       </c>
-      <c r="G18">
+      <c r="H20">
         <v>74</v>
       </c>
-      <c r="H18">
-        <f>G18/C18</f>
+      <c r="I20">
+        <f>H20/C20</f>
         <v>7.4</v>
       </c>
-      <c r="I18">
-        <f>(H18*500000)/60/60/24/30</f>
+      <c r="J20" s="1">
+        <f t="shared" si="3"/>
+        <v>0.36097560975609755</v>
+      </c>
+      <c r="K20">
+        <f>(I20*500000)/60/60/24/30</f>
         <v>1.4274691358024691</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19">
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
         <v>79</v>
       </c>
-      <c r="E19">
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="F21">
         <v>22</v>
       </c>
-      <c r="F19">
+      <c r="G21">
         <v>0.48499999999999999</v>
       </c>
-      <c r="G19">
+      <c r="H21">
         <v>40</v>
       </c>
-      <c r="H19">
-        <f>G19/C19</f>
+      <c r="I21">
+        <f>H21/C21</f>
         <v>40</v>
       </c>
-      <c r="I19">
-        <f>(H19*500000)/60/60/24/30</f>
+      <c r="J21" s="1">
+        <f>H21/D21</f>
+        <v>0.50632911392405067</v>
+      </c>
+      <c r="K21">
+        <f>(I21*500000)/60/60/24/30</f>
         <v>7.7160493827160499</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B21" t="s">
-        <v>1</v>
-      </c>
-      <c r="C21">
+      <c r="B23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23">
         <v>1000</v>
       </c>
-      <c r="D21">
+      <c r="D23">
         <v>3449</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="E23">
+        <f t="shared" ref="E23:E26" si="4">D23/C23</f>
+        <v>3.4489999999999998</v>
+      </c>
+      <c r="F23">
+        <v>5443</v>
+      </c>
+      <c r="G23">
+        <v>30828</v>
+      </c>
+      <c r="H23">
+        <f>605*60</f>
+        <v>36300</v>
+      </c>
+      <c r="I23">
+        <f>H23/C23</f>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="J23" s="1">
+        <f>H23/D23</f>
+        <v>10.52478979414323</v>
+      </c>
+      <c r="K23">
+        <f>(I23*500000)/60/60/24/30</f>
+        <v>7.0023148148148149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
-        <v>1</v>
-      </c>
-      <c r="C22">
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24">
         <v>100</v>
       </c>
-      <c r="D22">
+      <c r="D24">
         <v>355</v>
       </c>
-      <c r="E22">
+      <c r="E24">
+        <f t="shared" si="4"/>
+        <v>3.55</v>
+      </c>
+      <c r="F24">
         <v>297</v>
       </c>
-      <c r="F22">
+      <c r="G24">
         <v>243</v>
       </c>
-      <c r="G22">
+      <c r="H24">
         <f>(9*60)+21</f>
         <v>561</v>
       </c>
-      <c r="H22">
-        <f>G22/C22</f>
+      <c r="I24">
+        <f>H24/C24</f>
         <v>5.61</v>
       </c>
-      <c r="I22">
-        <f>(H22*500000)/60/60/24/30</f>
+      <c r="J24" s="1">
+        <f t="shared" ref="J24:J27" si="5">H24/D24</f>
+        <v>1.580281690140845</v>
+      </c>
+      <c r="K24">
+        <f>(I24*500000)/60/60/24/30</f>
         <v>1.082175925925926</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23">
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25">
         <v>50</v>
       </c>
-      <c r="D23">
+      <c r="D25">
         <v>189</v>
       </c>
-      <c r="E23">
+      <c r="E25">
+        <f t="shared" si="4"/>
+        <v>3.78</v>
+      </c>
+      <c r="F25">
         <v>227</v>
       </c>
-      <c r="F23">
+      <c r="G25">
         <v>95</v>
       </c>
-      <c r="G23">
+      <c r="H25">
         <f>(5*60)+40</f>
         <v>340</v>
       </c>
-      <c r="H23">
-        <f>G23/C23</f>
+      <c r="I25">
+        <f>H25/C25</f>
         <v>6.8</v>
       </c>
-      <c r="I23">
-        <f>(H23*500000)/60/60/24/30</f>
+      <c r="J25" s="1">
+        <f t="shared" si="5"/>
+        <v>1.7989417989417988</v>
+      </c>
+      <c r="K25">
+        <f>(I25*500000)/60/60/24/30</f>
         <v>1.3117283950617284</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>7</v>
       </c>
-      <c r="B24" t="s">
-        <v>1</v>
-      </c>
-      <c r="C24">
+      <c r="B26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26">
         <v>10</v>
       </c>
-      <c r="D24">
+      <c r="D26">
         <v>52</v>
       </c>
-      <c r="E24">
+      <c r="E26">
+        <f t="shared" si="4"/>
+        <v>5.2</v>
+      </c>
+      <c r="F26">
         <v>55</v>
       </c>
-      <c r="F24">
+      <c r="G26">
         <v>2</v>
       </c>
-      <c r="G24">
+      <c r="H26">
         <v>74</v>
       </c>
-      <c r="H24">
-        <f>G24/C24</f>
+      <c r="I26">
+        <f>H26/C26</f>
         <v>7.4</v>
       </c>
-      <c r="I24">
-        <f>(H24*500000)/60/60/24/30</f>
+      <c r="J26" s="1">
+        <f t="shared" si="5"/>
+        <v>1.4230769230769231</v>
+      </c>
+      <c r="K26">
+        <f>(I26*500000)/60/60/24/30</f>
         <v>1.4274691358024691</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>7</v>
       </c>
-      <c r="B25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25">
+      <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
         <v>16</v>
       </c>
-      <c r="E25">
+      <c r="E27">
+        <f>D27/C27</f>
+        <v>16</v>
+      </c>
+      <c r="F27">
         <v>22</v>
       </c>
-      <c r="F25">
+      <c r="G27">
         <v>0.44900000000000001</v>
       </c>
-      <c r="G25">
+      <c r="H27">
         <v>46</v>
       </c>
-      <c r="H25">
-        <f>G25/C25</f>
+      <c r="I27">
+        <f>H27/C27</f>
         <v>46</v>
       </c>
-      <c r="I25">
-        <f>(H25*500000)/60/60/24/30</f>
+      <c r="J27" s="1">
+        <f t="shared" si="5"/>
+        <v>2.875</v>
+      </c>
+      <c r="K27">
+        <f>(I27*500000)/60/60/24/30</f>
         <v>8.8734567901234573</v>
       </c>
     </row>

</xml_diff>